<commit_message>
Test to refactor Base page all test run Ok
</commit_message>
<xml_diff>
--- a/test_plan/Test Plan.xlsx
+++ b/test_plan/Test Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramingProjects\KatalonProjects\AcademiaQA_Katalon_YourStoreSite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramingProjects\CypressProjects\AcademiaQA_Cypress_YourStoreSite\test_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8383A438-395B-4C4A-BC5C-0DDB17D70EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D31AE18-AE80-4173-99CA-923803B433EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{E828D7EE-574E-4891-A092-A3D3FC4A54AE}"/>
   </bookViews>
@@ -281,9 +281,6 @@
     <t>Validar la seleccion de producto favorito</t>
   </si>
   <si>
-    <t>Visualización correcta del mensaje de comparar producto</t>
-  </si>
-  <si>
     <t>YS-12</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>Ver que el item fue eliminado del carrito de compras</t>
+  </si>
+  <si>
+    <t>Validar la visualización correcta del mensaje de comparar producto</t>
   </si>
 </sst>
 </file>
@@ -461,6 +461,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -490,13 +497,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -849,13 +849,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -869,9 +869,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
@@ -883,9 +883,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
@@ -897,9 +897,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
@@ -911,9 +911,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
@@ -925,13 +925,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -945,9 +945,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
@@ -959,9 +959,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
@@ -973,9 +973,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
@@ -987,9 +987,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1001,13 +1001,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1021,9 +1021,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1035,9 +1035,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
@@ -1049,9 +1049,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="5" t="s">
         <v>19</v>
       </c>
@@ -1063,9 +1063,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1077,13 +1077,13 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1097,9 +1097,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1111,9 +1111,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1125,9 +1125,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1145,18 +1145,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="C7:C11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1201,13 +1201,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1221,9 +1221,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1235,9 +1235,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1249,9 +1249,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
@@ -1263,13 +1263,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1283,9 +1283,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="5" t="s">
         <v>40</v>
       </c>
@@ -1297,9 +1297,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
@@ -1311,9 +1311,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="5" t="s">
         <v>53</v>
       </c>
@@ -1325,13 +1325,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1345,9 +1345,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
@@ -1359,9 +1359,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="5" t="s">
         <v>49</v>
       </c>
@@ -1373,9 +1373,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="5" t="s">
         <v>54</v>
       </c>
@@ -1387,13 +1387,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="18" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1407,9 +1407,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="16"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="5" t="s">
         <v>40</v>
       </c>
@@ -1421,9 +1421,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="16"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="5" t="s">
         <v>16</v>
       </c>
@@ -1435,9 +1435,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="16"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="5" t="s">
         <v>41</v>
       </c>
@@ -1449,9 +1449,9 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="17"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="5" t="s">
         <v>57</v>
       </c>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B412EA-237C-4DBE-9705-95B71194D3DE}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,13 +1526,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1546,9 +1546,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5" t="s">
         <v>61</v>
       </c>
@@ -1560,9 +1560,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="5" t="s">
         <v>69</v>
       </c>
@@ -1574,13 +1574,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1594,9 +1594,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="5" t="s">
         <v>61</v>
       </c>
@@ -1608,23 +1608,23 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5" t="s">
         <v>72</v>
       </c>
@@ -1636,9 +1636,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="5" t="s">
         <v>74</v>
       </c>
@@ -1650,13 +1650,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1670,9 +1670,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="5" t="s">
         <v>61</v>
       </c>
@@ -1684,23 +1684,23 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="5" t="s">
         <v>72</v>
       </c>
@@ -1712,9 +1712,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="5" t="s">
         <v>74</v>
       </c>
@@ -1726,9 +1726,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="5" t="s">
         <v>79</v>
       </c>
@@ -1740,14 +1740,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="C16" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>12</v>
@@ -1760,9 +1760,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="5" t="s">
         <v>61</v>
       </c>
@@ -1774,56 +1774,56 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="C21" s="18" t="s">
         <v>92</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>12</v>
@@ -1836,9 +1836,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="5" t="s">
         <v>61</v>
       </c>
@@ -1850,78 +1850,78 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="F25" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="19" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="10" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A26"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="C10:C15"/>
     <mergeCell ref="C16:C20"/>
     <mergeCell ref="C21:C26"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B21:B26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>